<commit_message>
a few changes for poster
</commit_message>
<xml_diff>
--- a/demos/modelPerformances.xlsx
+++ b/demos/modelPerformances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CS221-CoNBot\demos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C494286-E4F0-4CDB-B81F-64D6FDFCE4FF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6C634F-D3E0-4559-91C7-796C78D47291}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{3B771159-BD40-413C-9EA9-9AB09FFE75C1}"/>
   </bookViews>
@@ -403,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F9C976-0249-4DAA-B603-E60C3442872D}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H6" sqref="H6:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,60 +550,82 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>80</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>34</v>
+      </c>
+      <c r="E6">
+        <v>39</v>
+      </c>
+      <c r="F6">
+        <v>12</v>
+      </c>
+      <c r="G6">
+        <v>46</v>
+      </c>
+      <c r="H6">
+        <f>AVERAGE(C6:G6)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>154</v>
+      </c>
+      <c r="D7">
+        <v>185</v>
+      </c>
+      <c r="E7">
+        <v>144</v>
+      </c>
+      <c r="F7">
+        <v>200</v>
+      </c>
+      <c r="G7">
+        <v>169</v>
+      </c>
+      <c r="H7">
+        <f>AVERAGE(C7:G7)</f>
+        <v>170.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B11" s="1">
         <v>78</v>
       </c>
-      <c r="C6">
+      <c r="C11">
         <v>8</v>
       </c>
-      <c r="D6">
+      <c r="D11">
         <v>52</v>
       </c>
-      <c r="E6">
+      <c r="E11">
         <v>33</v>
       </c>
-      <c r="F6">
+      <c r="F11">
         <v>25</v>
       </c>
-      <c r="G6">
+      <c r="G11">
         <v>0</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
+      <c r="H11">
+        <f>AVERAGE(C11:G11)</f>
         <v>23.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1">
-        <v>80</v>
-      </c>
-      <c r="C7">
-        <v>9</v>
-      </c>
-      <c r="D7">
-        <v>34</v>
-      </c>
-      <c r="E7">
-        <v>39</v>
-      </c>
-      <c r="F7">
-        <v>12</v>
-      </c>
-      <c r="G7">
-        <v>46</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="0"/>
-        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="H2" formulaRange="1"/>
   </ignoredErrors>

</xml_diff>